<commit_message>
new polynomal calibration up to 75lb
</commit_message>
<xml_diff>
--- a/Calibration Data.xlsx
+++ b/Calibration Data.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorgatlin/Desktop/DataCollection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Allegion\Allegion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16755" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>Actual Force</t>
   </si>
@@ -39,6 +36,9 @@
   </si>
   <si>
     <t>Conductance</t>
+  </si>
+  <si>
+    <t>New Calibration</t>
   </si>
 </sst>
 </file>
@@ -86,6 +86,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -105,7 +108,14 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.4025136446985223"/>
+          <c:y val="2.8202115158636899E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -182,8 +192,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0265223097112861"/>
-                  <c:y val="-0.0320997375328084"/>
+                  <c:x val="-2.65223097112861E-2"/>
+                  <c:y val="-3.2099737532808398E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -223,28 +233,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>5.0E-6</c:v>
+                  <c:v>5.0000000000000004E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00027114967462039</c:v>
+                  <c:v>2.7114967462039046E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00277777777777778</c:v>
+                  <c:v>2.7777777777777779E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0062111801242236</c:v>
+                  <c:v>6.2111801242236021E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.00847457627118644</c:v>
+                  <c:v>8.4745762711864406E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0104166666666667</c:v>
+                  <c:v>1.0416666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0121951219512195</c:v>
+                  <c:v>1.2195121951219513E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0135135135135135</c:v>
+                  <c:v>1.3513513513513514E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -256,13 +266,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.94</c:v>
+                  <c:v>5.9399999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10.94</c:v>
@@ -271,13 +281,13 @@
                   <c:v>15.94</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.94</c:v>
+                  <c:v>20.939999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25.94</c:v>
+                  <c:v>25.939999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30.94</c:v>
+                  <c:v>30.939999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -292,11 +302,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1741880816"/>
-        <c:axId val="1707052800"/>
+        <c:axId val="196479288"/>
+        <c:axId val="196476544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1741880816"/>
+        <c:axId val="196479288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -372,6 +382,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -408,12 +419,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1707052800"/>
+        <c:crossAx val="196476544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1707052800"/>
+        <c:axId val="196476544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -489,6 +500,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -525,7 +537,548 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1741880816"/>
+        <c:crossAx val="196479288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.11914457567804025"/>
+                  <c:y val="-4.1666666666666669E-4"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$14:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000004E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.4889643463497452E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5105999097880024E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.1073205401563618E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.4117647058823521E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1536686663590217E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3410218586562963E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5767896562598548E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7427675148135237E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9062142584826535E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0354162426216162E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2070183182520412E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3212627669452184E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.4557956777996073E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.5647601949217745E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.6932399676811204E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.8026905829596414E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$14:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.9399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.94</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.939999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.939999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30.939999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35.94</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40.94</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.94</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50.94</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>55.94</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>60.94</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>65.94</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70.94</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>75.94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="456376344"/>
+        <c:axId val="456375952"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="456376344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Conductance</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="456375952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="456375952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Force (lb)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="456376344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -614,6 +1167,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1130,20 +1723,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1157,6 +2266,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1428,21 +2567,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" customWidth="1"/>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1456,7 +2595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1471,7 +2610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.1</v>
       </c>
@@ -1479,14 +2618,14 @@
         <v>3688</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C9" si="0">1/B3</f>
+        <f>1/B3</f>
         <v>2.7114967462039046E-4</v>
       </c>
       <c r="D3">
         <v>0.94</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.1000000000000001</v>
       </c>
@@ -1494,7 +2633,7 @@
         <v>360</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C3:C9" si="0">1/B4</f>
         <v>2.7777777777777779E-3</v>
       </c>
       <c r="D4">
@@ -1502,7 +2641,7 @@
         <v>5.9399999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.91</v>
       </c>
@@ -1518,7 +2657,7 @@
         <v>10.94</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2.2999999999999998</v>
       </c>
@@ -1534,7 +2673,7 @@
         <v>15.94</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2.5499999999999998</v>
       </c>
@@ -1550,7 +2689,7 @@
         <v>20.939999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2.75</v>
       </c>
@@ -1566,7 +2705,7 @@
         <v>25.939999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2.86</v>
       </c>
@@ -1580,6 +2719,295 @@
       <c r="D9">
         <f t="shared" si="1"/>
         <v>30.939999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>200000</v>
+      </c>
+      <c r="C14">
+        <f>1/B14</f>
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.4</v>
+      </c>
+      <c r="B15">
+        <v>1178</v>
+      </c>
+      <c r="C15">
+        <f>1/B15</f>
+        <v>8.4889643463497452E-4</v>
+      </c>
+      <c r="D15">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1.55</v>
+      </c>
+      <c r="B16">
+        <v>221.7</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:C21" si="2">1/B16</f>
+        <v>4.5105999097880024E-3</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:D30" si="3">D15+5</f>
+        <v>5.9399999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2.06</v>
+      </c>
+      <c r="B17">
+        <v>140.69999999999999</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="2"/>
+        <v>7.1073205401563618E-3</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="3"/>
+        <v>10.94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="B18">
+        <v>106.25</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="2"/>
+        <v>9.4117647058823521E-3</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="3"/>
+        <v>15.94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2.67</v>
+      </c>
+      <c r="B19">
+        <v>86.68</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="2"/>
+        <v>1.1536686663590217E-2</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="3"/>
+        <v>20.939999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2.85</v>
+      </c>
+      <c r="B20">
+        <v>74.569999999999993</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="2"/>
+        <v>1.3410218586562963E-2</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="3"/>
+        <v>25.939999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3.04</v>
+      </c>
+      <c r="B21">
+        <v>63.42</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="2"/>
+        <v>1.5767896562598548E-2</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="3"/>
+        <v>30.939999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3.17</v>
+      </c>
+      <c r="B22">
+        <v>57.38</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22:C25" si="4">1/B22</f>
+        <v>1.7427675148135237E-2</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="3"/>
+        <v>35.94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3.28</v>
+      </c>
+      <c r="B23">
+        <v>52.46</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="4"/>
+        <v>1.9062142584826535E-2</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="3"/>
+        <v>40.94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3.35</v>
+      </c>
+      <c r="B24">
+        <v>49.13</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="4"/>
+        <v>2.0354162426216162E-2</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="3"/>
+        <v>45.94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3.44</v>
+      </c>
+      <c r="B25">
+        <v>45.31</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="4"/>
+        <v>2.2070183182520412E-2</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="3"/>
+        <v>50.94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3.49</v>
+      </c>
+      <c r="B26">
+        <v>43.08</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26:C27" si="5">1/B26</f>
+        <v>2.3212627669452184E-2</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="3"/>
+        <v>55.94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3.55</v>
+      </c>
+      <c r="B27">
+        <v>40.72</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="5"/>
+        <v>2.4557956777996073E-2</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="3"/>
+        <v>60.94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3.62</v>
+      </c>
+      <c r="B28">
+        <v>38.99</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ref="C28" si="6">1/B28</f>
+        <v>2.5647601949217745E-2</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="3"/>
+        <v>65.94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3.64</v>
+      </c>
+      <c r="B29">
+        <v>37.130000000000003</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:C30" si="7">1/B29</f>
+        <v>2.6932399676811204E-2</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="3"/>
+        <v>70.94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3.68</v>
+      </c>
+      <c r="B30">
+        <v>35.68</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="7"/>
+        <v>2.8026905829596414E-2</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="3"/>
+        <v>75.94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>